<commit_message>
implement a function batch add a cron for every flow by read the config from excel ,if you don't fill the cell called cron ,appliction will remove the cron for the flow.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/PycharmProjects/azkaban_excel_yaml/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A0638F-253B-A74C-9E44-27E0215CF3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="scheduler" sheetId="4" r:id="rId4"/>
     <sheet name="ora2pg" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="105">
   <si>
     <t>Overview</t>
   </si>
@@ -52,6 +58,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -62,6 +69,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -74,6 +82,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -84,6 +93,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -96,6 +106,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -106,6 +117,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -118,6 +130,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -128,6 +141,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -145,9 +159,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>https://192.168.200.100:8443/</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -163,15 +174,6 @@
     <t>ods层贴源数据</t>
   </si>
   <si>
-    <t>dwd</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>ggg</t>
-  </si>
-  <si>
     <t>flow_name</t>
   </si>
   <si>
@@ -184,201 +186,102 @@
     <t>ORA2PG_JYDB_DELETEREC</t>
   </si>
   <si>
-    <t>"0 30 0 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_CT_SYSTEMCONST</t>
   </si>
   <si>
-    <t>"0 31 0 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_ANNOUNCEMENT</t>
   </si>
   <si>
-    <t>"0 30 1 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_ASSETALLOCATION</t>
   </si>
   <si>
-    <t>"0 31 1 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_BALANCESHEETNEW</t>
   </si>
   <si>
-    <t>"0 30 2 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_BONDPORTIFOLIODETAIL</t>
   </si>
   <si>
-    <t>"0 31 2 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_DIVIDEND</t>
   </si>
   <si>
-    <t>"0 30 3 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_FUNDARCHIVES</t>
   </si>
   <si>
-    <t>"0 31 3 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_FUNDARCHIVESATTACH</t>
   </si>
   <si>
-    <t>"0 30 4 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_FUNDMANAGERNEW</t>
   </si>
   <si>
-    <t>"0 31 4 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_FUNDPORTIFOLIODETAIL</t>
   </si>
   <si>
-    <t>"0 30 5 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_INCOMESTATEMENTNEW</t>
   </si>
   <si>
-    <t>"0 31 5 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_INTERIMBULLETIN</t>
   </si>
   <si>
-    <t>"0 30 6 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_INTERIMBULLETIN_SE</t>
   </si>
   <si>
-    <t>"0 31 6 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_INVESTADVISOROUTLINE</t>
   </si>
   <si>
-    <t>"0 30 7 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_INVESTINDUSTRY</t>
   </si>
   <si>
-    <t>"0 31 7 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_ISSUEANDLISTING</t>
   </si>
   <si>
-    <t>"0 30 8 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_KEYSTOCKPORTFOLIO</t>
   </si>
   <si>
-    <t>"0 31 8 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_MAINFINANCIALINDEX</t>
   </si>
   <si>
-    <t>"0 30 9 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_MMYIELDPERFORMANCE</t>
   </si>
   <si>
-    <t>"0 31 9 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_NETVALUE</t>
   </si>
   <si>
-    <t>"0 30 10 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_NETVALUEPERFORMANCE</t>
   </si>
   <si>
-    <t>"0 31 10 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_NETVALUEPERFORMANCEHIS</t>
   </si>
   <si>
-    <t>"0 30 11 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_QDIIASSETALLOCATION</t>
   </si>
   <si>
-    <t>"0 31 11 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_QDIIPORTFOLIOCHANGE</t>
   </si>
   <si>
-    <t>"0 30 12 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_QDIIPORTFOLIODETAIL</t>
   </si>
   <si>
-    <t>"0 31 12 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_QDIIPORTFOLIOINDUSTRY</t>
   </si>
   <si>
-    <t>"0 30 13 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_STOCKPORTFOLIOCHANGE</t>
   </si>
   <si>
-    <t>"0 31 13 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_STOCKPORTFOLIODETAIL</t>
   </si>
   <si>
-    <t>"0 30 14 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_MF_TRUSTEEOUTLINE</t>
   </si>
   <si>
-    <t>"0 31 14 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_SECUMAIN</t>
   </si>
   <si>
-    <t>"0 30 15 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_DONE</t>
   </si>
   <si>
-    <t>"0 31 15 * * ?"</t>
-  </si>
-  <si>
     <t>ORA2PG_DELETE_RECORDS</t>
   </si>
   <si>
-    <t>"0 30 16 * * ?"</t>
-  </si>
-  <si>
     <t>flow_desc</t>
   </si>
   <si>
@@ -521,19 +424,29 @@
   </si>
   <si>
     <t>ora2pg_all_done</t>
+  </si>
+  <si>
+    <t>https://192.168.31.36:18443/</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ora2pg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ora</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 0 4 1 12 ?</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +458,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -552,6 +466,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -559,6 +474,7 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -567,7 +483,8 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <family val="4"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -575,147 +492,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <family val="4"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="9"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <family val="4"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -728,188 +525,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1022,253 +639,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1284,7 +662,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1294,22 +672,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1337,62 +700,41 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1650,134 +992,133 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="10"/>
-    <col min="2" max="2" width="8.22222222222222" style="11" customWidth="1"/>
-    <col min="3" max="3" width="84.7777777777778" style="11" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="84.83203125" style="11" customWidth="1"/>
     <col min="4" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1" spans="1:4">
+    <row r="1" spans="1:4" ht="45" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" ht="44" customHeight="1" spans="1:4">
-      <c r="A2" s="15" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="1:4" ht="44" customHeight="1">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" ht="15.6" spans="1:4">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" ht="16">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="110.4" spans="1:4">
-      <c r="A5" s="22">
+    <row r="5" spans="1:4" ht="128">
+      <c r="A5" s="17">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="22">
         <v>44463</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="22"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="22"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="13.8" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:3">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1790,545 +1131,466 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://192.168.200.100:8443/" tooltip="https://192.168.200.100:8443/"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://192.168.31.36:8443/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8333333333333" defaultRowHeight="13.8" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:2">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>20</v>
+      <c r="A3" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="39.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="12.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>27</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>45</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>47</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>51</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>55</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>59</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
+      <c r="A22" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>69</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>71</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>73</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>75</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>77</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>79</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>85</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>87</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>89</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C34" s="29"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A85" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.8333333333333" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="39.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="39.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="44.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="37.8333333333333" customWidth="1"/>
-    <col min="6" max="6" width="12.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="9.83333333333333" customWidth="1"/>
-    <col min="8" max="8" width="82.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="255.833333333333" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="82.33203125" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E2" t="str">
         <f>LOWER(B2)</f>
         <v>ora2pg_jydb_deleterec</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H2" s="5" t="str">
         <f>"sh ${sync_shell} "&amp;MID(E2,8,LEN(E2)-7)&amp;" ${dt}"</f>
@@ -2337,42 +1599,42 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I3" s="5" t="str">
         <f>E2</f>
         <v>ora2pg_jydb_deleterec</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:9">
+    <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H4" s="5" t="str">
         <f t="shared" ref="H4" si="0">"sh ${sync_shell} "&amp;MID(E4,8,LEN(E4)-7)&amp;" ${dt}"</f>
@@ -2382,44 +1644,44 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I5" s="5" t="str">
         <f>E4</f>
         <v>ora2pg_ct_systemconst</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ref="E6" si="1">LOWER(B6)</f>
         <v>ora2pg_mf_announcement</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H6" s="5" t="str">
         <f t="shared" ref="H6" si="2">"sh ${sync_shell} "&amp;MID(E6,8,LEN(E6)-7)&amp;" ${dt}"</f>
@@ -2428,42 +1690,42 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I7" s="5" t="str">
         <f t="shared" ref="I7" si="3">E6</f>
         <v>ora2pg_mf_announcement</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" ref="E8" si="4">LOWER(B8)</f>
         <v>ora2pg_mf_assetallocation</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H8" s="5" t="str">
         <f t="shared" ref="H8" si="5">"sh ${sync_shell} "&amp;MID(E8,8,LEN(E8)-7)&amp;" ${dt}"</f>
@@ -2472,42 +1734,42 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I9" s="5" t="str">
         <f t="shared" ref="I9" si="6">E8</f>
         <v>ora2pg_mf_assetallocation</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ref="E10" si="7">LOWER(B10)</f>
         <v>ora2pg_mf_balancesheetnew</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H10" s="5" t="str">
         <f t="shared" ref="H10" si="8">"sh ${sync_shell} "&amp;MID(E10,8,LEN(E10)-7)&amp;" ${dt}"</f>
@@ -2516,42 +1778,42 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I11" s="5" t="str">
         <f t="shared" ref="I11" si="9">E10</f>
         <v>ora2pg_mf_balancesheetnew</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" ref="E12" si="10">LOWER(B12)</f>
         <v>ora2pg_mf_bondportifoliodetail</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H12" s="5" t="str">
         <f t="shared" ref="H12" si="11">"sh ${sync_shell} "&amp;MID(E12,8,LEN(E12)-7)&amp;" ${dt}"</f>
@@ -2560,42 +1822,42 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I13" s="5" t="str">
         <f t="shared" ref="I13" si="12">E12</f>
         <v>ora2pg_mf_bondportifoliodetail</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" ref="E14" si="13">LOWER(B14)</f>
         <v>ora2pg_mf_dividend</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H14" s="5" t="str">
         <f t="shared" ref="H14" si="14">"sh ${sync_shell} "&amp;MID(E14,8,LEN(E14)-7)&amp;" ${dt}"</f>
@@ -2604,42 +1866,42 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I15" s="5" t="str">
         <f t="shared" ref="I15" si="15">E14</f>
         <v>ora2pg_mf_dividend</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" ref="E16" si="16">LOWER(B16)</f>
         <v>ora2pg_mf_fundarchives</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H16" s="5" t="str">
         <f t="shared" ref="H16" si="17">"sh ${sync_shell} "&amp;MID(E16,8,LEN(E16)-7)&amp;" ${dt}"</f>
@@ -2648,42 +1910,42 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I17" s="5" t="str">
         <f t="shared" ref="I17" si="18">E16</f>
         <v>ora2pg_mf_fundarchives</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" ref="E18" si="19">LOWER(B18)</f>
         <v>ora2pg_mf_fundarchivesattach</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H18" s="5" t="str">
         <f t="shared" ref="H18" si="20">"sh ${sync_shell} "&amp;MID(E18,8,LEN(E18)-7)&amp;" ${dt}"</f>
@@ -2692,42 +1954,42 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I19" s="5" t="str">
         <f t="shared" ref="I19" si="21">E18</f>
         <v>ora2pg_mf_fundarchivesattach</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" ref="E20" si="22">LOWER(B20)</f>
         <v>ora2pg_mf_fundmanagernew</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H20" s="5" t="str">
         <f t="shared" ref="H20" si="23">"sh ${sync_shell} "&amp;MID(E20,8,LEN(E20)-7)&amp;" ${dt}"</f>
@@ -2736,42 +1998,42 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I21" s="5" t="str">
         <f t="shared" ref="I21" si="24">E20</f>
         <v>ora2pg_mf_fundmanagernew</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" ref="E22" si="25">LOWER(B22)</f>
         <v>ora2pg_mf_fundportifoliodetail</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H22" s="5" t="str">
         <f t="shared" ref="H22" si="26">"sh ${sync_shell} "&amp;MID(E22,8,LEN(E22)-7)&amp;" ${dt}"</f>
@@ -2780,42 +2042,42 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I23" s="5" t="str">
         <f t="shared" ref="I23" si="27">E22</f>
         <v>ora2pg_mf_fundportifoliodetail</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" ref="E24" si="28">LOWER(B24)</f>
         <v>ora2pg_mf_incomestatementnew</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H24" s="5" t="str">
         <f t="shared" ref="H24" si="29">"sh ${sync_shell} "&amp;MID(E24,8,LEN(E24)-7)&amp;" ${dt}"</f>
@@ -2824,42 +2086,42 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I25" s="5" t="str">
         <f t="shared" ref="I25" si="30">E24</f>
         <v>ora2pg_mf_incomestatementnew</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" ref="E26" si="31">LOWER(B26)</f>
         <v>ora2pg_mf_interimbulletin</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H26" s="5" t="str">
         <f t="shared" ref="H26" si="32">"sh ${sync_shell} "&amp;MID(E26,8,LEN(E26)-7)&amp;" ${dt}"</f>
@@ -2868,42 +2130,42 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I27" s="5" t="str">
         <f t="shared" ref="I27" si="33">E26</f>
         <v>ora2pg_mf_interimbulletin</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" ref="E28" si="34">LOWER(B28)</f>
         <v>ora2pg_mf_interimbulletin_se</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H28" s="5" t="str">
         <f t="shared" ref="H28" si="35">"sh ${sync_shell} "&amp;MID(E28,8,LEN(E28)-7)&amp;" ${dt}"</f>
@@ -2912,42 +2174,42 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I29" s="5" t="str">
         <f t="shared" ref="I29" si="36">E28</f>
         <v>ora2pg_mf_interimbulletin_se</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" ref="E30" si="37">LOWER(B30)</f>
         <v>ora2pg_mf_investadvisoroutline</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H30" s="5" t="str">
         <f t="shared" ref="H30" si="38">"sh ${sync_shell} "&amp;MID(E30,8,LEN(E30)-7)&amp;" ${dt}"</f>
@@ -2956,42 +2218,42 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I31" s="5" t="str">
         <f t="shared" ref="I31" si="39">E30</f>
         <v>ora2pg_mf_investadvisoroutline</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" ref="E32" si="40">LOWER(B32)</f>
         <v>ora2pg_mf_investindustry</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H32" s="5" t="str">
         <f t="shared" ref="H32" si="41">"sh ${sync_shell} "&amp;MID(E32,8,LEN(E32)-7)&amp;" ${dt}"</f>
@@ -3000,42 +2262,42 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I33" s="5" t="str">
         <f t="shared" ref="I33" si="42">E32</f>
         <v>ora2pg_mf_investindustry</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" ref="E34" si="43">LOWER(B34)</f>
         <v>ora2pg_mf_issueandlisting</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H34" s="5" t="str">
         <f t="shared" ref="H34" si="44">"sh ${sync_shell} "&amp;MID(E34,8,LEN(E34)-7)&amp;" ${dt}"</f>
@@ -3044,42 +2306,42 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I35" s="5" t="str">
         <f t="shared" ref="I35" si="45">E34</f>
         <v>ora2pg_mf_issueandlisting</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" ref="E36" si="46">LOWER(B36)</f>
         <v>ora2pg_mf_keystockportfolio</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H36" s="5" t="str">
         <f t="shared" ref="H36" si="47">"sh ${sync_shell} "&amp;MID(E36,8,LEN(E36)-7)&amp;" ${dt}"</f>
@@ -3088,42 +2350,42 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I37" s="5" t="str">
         <f t="shared" ref="I37" si="48">E36</f>
         <v>ora2pg_mf_keystockportfolio</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" ref="E38" si="49">LOWER(B38)</f>
         <v>ora2pg_mf_mainfinancialindex</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H38" s="5" t="str">
         <f t="shared" ref="H38" si="50">"sh ${sync_shell} "&amp;MID(E38,8,LEN(E38)-7)&amp;" ${dt}"</f>
@@ -3132,42 +2394,42 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I39" s="5" t="str">
         <f t="shared" ref="I39" si="51">E38</f>
         <v>ora2pg_mf_mainfinancialindex</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ref="E40" si="52">LOWER(B40)</f>
         <v>ora2pg_mf_mmyieldperformance</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H40" s="5" t="str">
         <f t="shared" ref="H40" si="53">"sh ${sync_shell} "&amp;MID(E40,8,LEN(E40)-7)&amp;" ${dt}"</f>
@@ -3176,42 +2438,42 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I41" s="5" t="str">
         <f t="shared" ref="I41" si="54">E40</f>
         <v>ora2pg_mf_mmyieldperformance</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" ref="E42" si="55">LOWER(B42)</f>
         <v>ora2pg_mf_netvalue</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H42" s="5" t="str">
         <f t="shared" ref="H42" si="56">"sh ${sync_shell} "&amp;MID(E42,8,LEN(E42)-7)&amp;" ${dt}"</f>
@@ -3220,42 +2482,42 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I43" s="5" t="str">
         <f t="shared" ref="I43" si="57">E42</f>
         <v>ora2pg_mf_netvalue</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" ref="E44" si="58">LOWER(B44)</f>
         <v>ora2pg_mf_netvalueperformance</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H44" s="5" t="str">
         <f t="shared" ref="H44" si="59">"sh ${sync_shell} "&amp;MID(E44,8,LEN(E44)-7)&amp;" ${dt}"</f>
@@ -3264,42 +2526,42 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I45" s="5" t="str">
         <f t="shared" ref="I45" si="60">E44</f>
         <v>ora2pg_mf_netvalueperformance</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" ref="E46" si="61">LOWER(B46)</f>
         <v>ora2pg_mf_netvalueperformancehis</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H46" s="5" t="str">
         <f t="shared" ref="H46" si="62">"sh ${sync_shell} "&amp;MID(E46,8,LEN(E46)-7)&amp;" ${dt}"</f>
@@ -3308,42 +2570,42 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I47" s="5" t="str">
         <f t="shared" ref="I47" si="63">E46</f>
         <v>ora2pg_mf_netvalueperformancehis</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" ref="E48" si="64">LOWER(B48)</f>
         <v>ora2pg_mf_qdiiassetallocation</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H48" s="5" t="str">
         <f t="shared" ref="H48" si="65">"sh ${sync_shell} "&amp;MID(E48,8,LEN(E48)-7)&amp;" ${dt}"</f>
@@ -3352,42 +2614,42 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I49" s="5" t="str">
         <f t="shared" ref="I49" si="66">E48</f>
         <v>ora2pg_mf_qdiiassetallocation</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" ref="E50" si="67">LOWER(B50)</f>
         <v>ora2pg_mf_qdiiportfoliochange</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H50" s="5" t="str">
         <f t="shared" ref="H50" si="68">"sh ${sync_shell} "&amp;MID(E50,8,LEN(E50)-7)&amp;" ${dt}"</f>
@@ -3396,42 +2658,42 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I51" s="5" t="str">
         <f t="shared" ref="I51" si="69">E50</f>
         <v>ora2pg_mf_qdiiportfoliochange</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" ref="E52" si="70">LOWER(B52)</f>
         <v>ora2pg_mf_qdiiportfoliodetail</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H52" s="5" t="str">
         <f t="shared" ref="H52" si="71">"sh ${sync_shell} "&amp;MID(E52,8,LEN(E52)-7)&amp;" ${dt}"</f>
@@ -3440,42 +2702,42 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I53" s="5" t="str">
         <f t="shared" ref="I53" si="72">E52</f>
         <v>ora2pg_mf_qdiiportfoliodetail</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" ref="E54" si="73">LOWER(B54)</f>
         <v>ora2pg_mf_qdiiportfolioindustry</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H54" s="5" t="str">
         <f t="shared" ref="H54" si="74">"sh ${sync_shell} "&amp;MID(E54,8,LEN(E54)-7)&amp;" ${dt}"</f>
@@ -3484,42 +2746,42 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I55" s="5" t="str">
         <f t="shared" ref="I55" si="75">E54</f>
         <v>ora2pg_mf_qdiiportfolioindustry</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" ref="E56" si="76">LOWER(B56)</f>
         <v>ora2pg_mf_stockportfoliochange</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H56" s="5" t="str">
         <f t="shared" ref="H56" si="77">"sh ${sync_shell} "&amp;MID(E56,8,LEN(E56)-7)&amp;" ${dt}"</f>
@@ -3528,42 +2790,42 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I57" s="5" t="str">
         <f t="shared" ref="I57" si="78">E56</f>
         <v>ora2pg_mf_stockportfoliochange</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" ref="E58" si="79">LOWER(B58)</f>
         <v>ora2pg_mf_stockportfoliodetail</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H58" s="5" t="str">
         <f t="shared" ref="H58" si="80">"sh ${sync_shell} "&amp;MID(E58,8,LEN(E58)-7)&amp;" ${dt}"</f>
@@ -3572,42 +2834,42 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I59" s="5" t="str">
         <f t="shared" ref="I59" si="81">E58</f>
         <v>ora2pg_mf_stockportfoliodetail</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" ref="E60" si="82">LOWER(B60)</f>
         <v>ora2pg_mf_trusteeoutline</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H60" s="5" t="str">
         <f t="shared" ref="H60" si="83">"sh ${sync_shell} "&amp;MID(E60,8,LEN(E60)-7)&amp;" ${dt}"</f>
@@ -3616,42 +2878,42 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I61" s="5" t="str">
         <f t="shared" ref="I61" si="84">E60</f>
         <v>ora2pg_mf_trusteeoutline</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" ref="E62" si="85">LOWER(B62)</f>
         <v>ora2pg_secumain</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H62" s="5" t="str">
         <f t="shared" ref="H62" si="86">"sh ${sync_shell} "&amp;MID(E62,8,LEN(E62)-7)&amp;" ${dt}"</f>
@@ -3660,41 +2922,41 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="5" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I63" s="5" t="str">
         <f t="shared" ref="I63" si="87">E62</f>
         <v>ora2pg_secumain</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E64" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H64" s="5" t="str">
         <f>"sh ${check_script} ora2pg "&amp;UPPER(MID(E64,1,LEN(E64)-5))&amp;" ${dt}"</f>
@@ -3703,17 +2965,17 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H65" s="5" t="str">
         <f t="shared" ref="H65:H97" si="88">"sh ${check_script} ora2pg "&amp;UPPER(MID(E65,1,LEN(E65)-5))&amp;" ${dt}"</f>
@@ -3722,17 +2984,17 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H66" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3741,17 +3003,17 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H67" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3760,17 +3022,17 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H68" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3779,17 +3041,17 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H69" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3798,17 +3060,17 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H70" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3817,17 +3079,17 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H71" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3836,17 +3098,17 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H72" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3855,17 +3117,17 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H73" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3874,17 +3136,17 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H74" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3893,17 +3155,17 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H75" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3912,17 +3174,17 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H76" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3931,17 +3193,17 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H77" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3950,17 +3212,17 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H78" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3969,17 +3231,17 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H79" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3988,283 +3250,283 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H80" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_ISSUEANDLISTING ${dt}</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H81" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_KEYSTOCKPORTFOLIO ${dt}</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H82" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_MAINFINANCIALINDEX ${dt}</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H83" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_MMYIELDPERFORMANCE ${dt}</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H84" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_NETVALUE ${dt}</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H85" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_NETVALUEPERFORMANCE ${dt}</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H86" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_NETVALUEPERFORMANCEHIS ${dt}</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H87" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_QDIIASSETALLOCATION ${dt}</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H88" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_QDIIPORTFOLIOCHANGE ${dt}</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H89" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_QDIIPORTFOLIODETAIL ${dt}</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H90" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_QDIIPORTFOLIOINDUSTRY ${dt}</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:9">
       <c r="A91" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H91" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_STOCKPORTFOLIOCHANGE ${dt}</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:9">
       <c r="A92" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H92" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_STOCKPORTFOLIODETAIL ${dt}</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H93" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_MF_TRUSTEEOUTLINE ${dt}</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H94" s="5" t="str">
         <f t="shared" si="88"/>
@@ -4273,40 +3535,40 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="3" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="I95" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H96" s="5" t="str">
         <f t="shared" si="88"/>
@@ -4315,50 +3577,50 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="3" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H97" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_DELETE_RE ${dt}</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="3" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="H98" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I98" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I98" s="3" t="s">
-        <v>136</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integration the two scripts as a application 1.generator.py read excel and generate flow files and compress they into zipfile 2.generator.py invoke scheduler.py to create project ,upload zipfile to Azkaban WebUI and schedule the flow which has cron. Unschedule flow which no cron.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/PycharmProjects/azkaban_excel_yaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A0638F-253B-A74C-9E44-27E0215CF3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9463DD0B-9711-DA49-B3A7-12074B0FF553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -168,12 +168,6 @@
     <t>project_desc</t>
   </si>
   <si>
-    <t>ods</t>
-  </si>
-  <si>
-    <t>ods层贴源数据</t>
-  </si>
-  <si>
     <t>flow_name</t>
   </si>
   <si>
@@ -439,6 +433,14 @@
   </si>
   <si>
     <t>0 0 4 1 12 ?</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>base_dir</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Users/jing/jbf/jobs/</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1105,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C45"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1116,9 +1118,10 @@
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1128,16 +1131,22 @@
       <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1151,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15"/>
@@ -1172,19 +1181,11 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>103</v>
+      <c r="A2" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1197,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -1213,308 +1214,308 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="29"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="29"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="29"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="29"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C34" s="29"/>
     </row>
@@ -1551,46 +1552,46 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" t="str">
         <f>LOWER(B2)</f>
         <v>ora2pg_jydb_deleterec</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="5" t="str">
         <f>"sh ${sync_shell} "&amp;MID(E2,8,LEN(E2)-7)&amp;" ${dt}"</f>
@@ -1599,20 +1600,20 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3" s="5" t="str">
         <f>E2</f>
@@ -1621,20 +1622,20 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H4" s="5" t="str">
         <f t="shared" ref="H4" si="0">"sh ${sync_shell} "&amp;MID(E4,8,LEN(E4)-7)&amp;" ${dt}"</f>
@@ -1644,22 +1645,22 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I5" s="5" t="str">
         <f>E4</f>
@@ -1668,20 +1669,20 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ref="E6" si="1">LOWER(B6)</f>
         <v>ora2pg_mf_announcement</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H6" s="5" t="str">
         <f t="shared" ref="H6" si="2">"sh ${sync_shell} "&amp;MID(E6,8,LEN(E6)-7)&amp;" ${dt}"</f>
@@ -1690,20 +1691,20 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I7" s="5" t="str">
         <f t="shared" ref="I7" si="3">E6</f>
@@ -1712,20 +1713,20 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" ref="E8" si="4">LOWER(B8)</f>
         <v>ora2pg_mf_assetallocation</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H8" s="5" t="str">
         <f t="shared" ref="H8" si="5">"sh ${sync_shell} "&amp;MID(E8,8,LEN(E8)-7)&amp;" ${dt}"</f>
@@ -1734,20 +1735,20 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9" s="5" t="str">
         <f t="shared" ref="I9" si="6">E8</f>
@@ -1756,20 +1757,20 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ref="E10" si="7">LOWER(B10)</f>
         <v>ora2pg_mf_balancesheetnew</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H10" s="5" t="str">
         <f t="shared" ref="H10" si="8">"sh ${sync_shell} "&amp;MID(E10,8,LEN(E10)-7)&amp;" ${dt}"</f>
@@ -1778,20 +1779,20 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I11" s="5" t="str">
         <f t="shared" ref="I11" si="9">E10</f>
@@ -1800,20 +1801,20 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" ref="E12" si="10">LOWER(B12)</f>
         <v>ora2pg_mf_bondportifoliodetail</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H12" s="5" t="str">
         <f t="shared" ref="H12" si="11">"sh ${sync_shell} "&amp;MID(E12,8,LEN(E12)-7)&amp;" ${dt}"</f>
@@ -1822,20 +1823,20 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I13" s="5" t="str">
         <f t="shared" ref="I13" si="12">E12</f>
@@ -1844,20 +1845,20 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" ref="E14" si="13">LOWER(B14)</f>
         <v>ora2pg_mf_dividend</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H14" s="5" t="str">
         <f t="shared" ref="H14" si="14">"sh ${sync_shell} "&amp;MID(E14,8,LEN(E14)-7)&amp;" ${dt}"</f>
@@ -1866,20 +1867,20 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I15" s="5" t="str">
         <f t="shared" ref="I15" si="15">E14</f>
@@ -1888,20 +1889,20 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" ref="E16" si="16">LOWER(B16)</f>
         <v>ora2pg_mf_fundarchives</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H16" s="5" t="str">
         <f t="shared" ref="H16" si="17">"sh ${sync_shell} "&amp;MID(E16,8,LEN(E16)-7)&amp;" ${dt}"</f>
@@ -1910,20 +1911,20 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I17" s="5" t="str">
         <f t="shared" ref="I17" si="18">E16</f>
@@ -1932,20 +1933,20 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" ref="E18" si="19">LOWER(B18)</f>
         <v>ora2pg_mf_fundarchivesattach</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H18" s="5" t="str">
         <f t="shared" ref="H18" si="20">"sh ${sync_shell} "&amp;MID(E18,8,LEN(E18)-7)&amp;" ${dt}"</f>
@@ -1954,20 +1955,20 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I19" s="5" t="str">
         <f t="shared" ref="I19" si="21">E18</f>
@@ -1976,20 +1977,20 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" ref="E20" si="22">LOWER(B20)</f>
         <v>ora2pg_mf_fundmanagernew</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H20" s="5" t="str">
         <f t="shared" ref="H20" si="23">"sh ${sync_shell} "&amp;MID(E20,8,LEN(E20)-7)&amp;" ${dt}"</f>
@@ -1998,20 +1999,20 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I21" s="5" t="str">
         <f t="shared" ref="I21" si="24">E20</f>
@@ -2020,20 +2021,20 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" ref="E22" si="25">LOWER(B22)</f>
         <v>ora2pg_mf_fundportifoliodetail</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" s="5" t="str">
         <f t="shared" ref="H22" si="26">"sh ${sync_shell} "&amp;MID(E22,8,LEN(E22)-7)&amp;" ${dt}"</f>
@@ -2042,20 +2043,20 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I23" s="5" t="str">
         <f t="shared" ref="I23" si="27">E22</f>
@@ -2064,20 +2065,20 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" ref="E24" si="28">LOWER(B24)</f>
         <v>ora2pg_mf_incomestatementnew</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H24" s="5" t="str">
         <f t="shared" ref="H24" si="29">"sh ${sync_shell} "&amp;MID(E24,8,LEN(E24)-7)&amp;" ${dt}"</f>
@@ -2086,20 +2087,20 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I25" s="5" t="str">
         <f t="shared" ref="I25" si="30">E24</f>
@@ -2108,20 +2109,20 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" ref="E26" si="31">LOWER(B26)</f>
         <v>ora2pg_mf_interimbulletin</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H26" s="5" t="str">
         <f t="shared" ref="H26" si="32">"sh ${sync_shell} "&amp;MID(E26,8,LEN(E26)-7)&amp;" ${dt}"</f>
@@ -2130,20 +2131,20 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I27" s="5" t="str">
         <f t="shared" ref="I27" si="33">E26</f>
@@ -2152,20 +2153,20 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" ref="E28" si="34">LOWER(B28)</f>
         <v>ora2pg_mf_interimbulletin_se</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H28" s="5" t="str">
         <f t="shared" ref="H28" si="35">"sh ${sync_shell} "&amp;MID(E28,8,LEN(E28)-7)&amp;" ${dt}"</f>
@@ -2174,20 +2175,20 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I29" s="5" t="str">
         <f t="shared" ref="I29" si="36">E28</f>
@@ -2196,20 +2197,20 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" ref="E30" si="37">LOWER(B30)</f>
         <v>ora2pg_mf_investadvisoroutline</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H30" s="5" t="str">
         <f t="shared" ref="H30" si="38">"sh ${sync_shell} "&amp;MID(E30,8,LEN(E30)-7)&amp;" ${dt}"</f>
@@ -2218,20 +2219,20 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I31" s="5" t="str">
         <f t="shared" ref="I31" si="39">E30</f>
@@ -2240,20 +2241,20 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" ref="E32" si="40">LOWER(B32)</f>
         <v>ora2pg_mf_investindustry</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H32" s="5" t="str">
         <f t="shared" ref="H32" si="41">"sh ${sync_shell} "&amp;MID(E32,8,LEN(E32)-7)&amp;" ${dt}"</f>
@@ -2262,20 +2263,20 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I33" s="5" t="str">
         <f t="shared" ref="I33" si="42">E32</f>
@@ -2284,20 +2285,20 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" ref="E34" si="43">LOWER(B34)</f>
         <v>ora2pg_mf_issueandlisting</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H34" s="5" t="str">
         <f t="shared" ref="H34" si="44">"sh ${sync_shell} "&amp;MID(E34,8,LEN(E34)-7)&amp;" ${dt}"</f>
@@ -2306,20 +2307,20 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I35" s="5" t="str">
         <f t="shared" ref="I35" si="45">E34</f>
@@ -2328,20 +2329,20 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" ref="E36" si="46">LOWER(B36)</f>
         <v>ora2pg_mf_keystockportfolio</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H36" s="5" t="str">
         <f t="shared" ref="H36" si="47">"sh ${sync_shell} "&amp;MID(E36,8,LEN(E36)-7)&amp;" ${dt}"</f>
@@ -2350,20 +2351,20 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I37" s="5" t="str">
         <f t="shared" ref="I37" si="48">E36</f>
@@ -2372,20 +2373,20 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" ref="E38" si="49">LOWER(B38)</f>
         <v>ora2pg_mf_mainfinancialindex</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H38" s="5" t="str">
         <f t="shared" ref="H38" si="50">"sh ${sync_shell} "&amp;MID(E38,8,LEN(E38)-7)&amp;" ${dt}"</f>
@@ -2394,20 +2395,20 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I39" s="5" t="str">
         <f t="shared" ref="I39" si="51">E38</f>
@@ -2416,20 +2417,20 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ref="E40" si="52">LOWER(B40)</f>
         <v>ora2pg_mf_mmyieldperformance</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H40" s="5" t="str">
         <f t="shared" ref="H40" si="53">"sh ${sync_shell} "&amp;MID(E40,8,LEN(E40)-7)&amp;" ${dt}"</f>
@@ -2438,20 +2439,20 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I41" s="5" t="str">
         <f t="shared" ref="I41" si="54">E40</f>
@@ -2460,20 +2461,20 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" ref="E42" si="55">LOWER(B42)</f>
         <v>ora2pg_mf_netvalue</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H42" s="5" t="str">
         <f t="shared" ref="H42" si="56">"sh ${sync_shell} "&amp;MID(E42,8,LEN(E42)-7)&amp;" ${dt}"</f>
@@ -2482,20 +2483,20 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I43" s="5" t="str">
         <f t="shared" ref="I43" si="57">E42</f>
@@ -2504,20 +2505,20 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" ref="E44" si="58">LOWER(B44)</f>
         <v>ora2pg_mf_netvalueperformance</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H44" s="5" t="str">
         <f t="shared" ref="H44" si="59">"sh ${sync_shell} "&amp;MID(E44,8,LEN(E44)-7)&amp;" ${dt}"</f>
@@ -2526,20 +2527,20 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I45" s="5" t="str">
         <f t="shared" ref="I45" si="60">E44</f>
@@ -2548,20 +2549,20 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" ref="E46" si="61">LOWER(B46)</f>
         <v>ora2pg_mf_netvalueperformancehis</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H46" s="5" t="str">
         <f t="shared" ref="H46" si="62">"sh ${sync_shell} "&amp;MID(E46,8,LEN(E46)-7)&amp;" ${dt}"</f>
@@ -2570,20 +2571,20 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I47" s="5" t="str">
         <f t="shared" ref="I47" si="63">E46</f>
@@ -2592,20 +2593,20 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" ref="E48" si="64">LOWER(B48)</f>
         <v>ora2pg_mf_qdiiassetallocation</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H48" s="5" t="str">
         <f t="shared" ref="H48" si="65">"sh ${sync_shell} "&amp;MID(E48,8,LEN(E48)-7)&amp;" ${dt}"</f>
@@ -2614,20 +2615,20 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I49" s="5" t="str">
         <f t="shared" ref="I49" si="66">E48</f>
@@ -2636,20 +2637,20 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" ref="E50" si="67">LOWER(B50)</f>
         <v>ora2pg_mf_qdiiportfoliochange</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H50" s="5" t="str">
         <f t="shared" ref="H50" si="68">"sh ${sync_shell} "&amp;MID(E50,8,LEN(E50)-7)&amp;" ${dt}"</f>
@@ -2658,20 +2659,20 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I51" s="5" t="str">
         <f t="shared" ref="I51" si="69">E50</f>
@@ -2680,20 +2681,20 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" ref="E52" si="70">LOWER(B52)</f>
         <v>ora2pg_mf_qdiiportfoliodetail</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H52" s="5" t="str">
         <f t="shared" ref="H52" si="71">"sh ${sync_shell} "&amp;MID(E52,8,LEN(E52)-7)&amp;" ${dt}"</f>
@@ -2702,20 +2703,20 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I53" s="5" t="str">
         <f t="shared" ref="I53" si="72">E52</f>
@@ -2724,20 +2725,20 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" ref="E54" si="73">LOWER(B54)</f>
         <v>ora2pg_mf_qdiiportfolioindustry</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H54" s="5" t="str">
         <f t="shared" ref="H54" si="74">"sh ${sync_shell} "&amp;MID(E54,8,LEN(E54)-7)&amp;" ${dt}"</f>
@@ -2746,20 +2747,20 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I55" s="5" t="str">
         <f t="shared" ref="I55" si="75">E54</f>
@@ -2768,20 +2769,20 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" ref="E56" si="76">LOWER(B56)</f>
         <v>ora2pg_mf_stockportfoliochange</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H56" s="5" t="str">
         <f t="shared" ref="H56" si="77">"sh ${sync_shell} "&amp;MID(E56,8,LEN(E56)-7)&amp;" ${dt}"</f>
@@ -2790,20 +2791,20 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I57" s="5" t="str">
         <f t="shared" ref="I57" si="78">E56</f>
@@ -2812,20 +2813,20 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" ref="E58" si="79">LOWER(B58)</f>
         <v>ora2pg_mf_stockportfoliodetail</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H58" s="5" t="str">
         <f t="shared" ref="H58" si="80">"sh ${sync_shell} "&amp;MID(E58,8,LEN(E58)-7)&amp;" ${dt}"</f>
@@ -2834,20 +2835,20 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I59" s="5" t="str">
         <f t="shared" ref="I59" si="81">E58</f>
@@ -2856,20 +2857,20 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" ref="E60" si="82">LOWER(B60)</f>
         <v>ora2pg_mf_trusteeoutline</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H60" s="5" t="str">
         <f t="shared" ref="H60" si="83">"sh ${sync_shell} "&amp;MID(E60,8,LEN(E60)-7)&amp;" ${dt}"</f>
@@ -2878,20 +2879,20 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I61" s="5" t="str">
         <f t="shared" ref="I61" si="84">E60</f>
@@ -2900,20 +2901,20 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" ref="E62" si="85">LOWER(B62)</f>
         <v>ora2pg_secumain</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H62" s="5" t="str">
         <f t="shared" ref="H62" si="86">"sh ${sync_shell} "&amp;MID(E62,8,LEN(E62)-7)&amp;" ${dt}"</f>
@@ -2922,20 +2923,20 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I63" s="5" t="str">
         <f t="shared" ref="I63" si="87">E62</f>
@@ -2944,19 +2945,19 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H64" s="5" t="str">
         <f>"sh ${check_script} ora2pg "&amp;UPPER(MID(E64,1,LEN(E64)-5))&amp;" ${dt}"</f>
@@ -2965,17 +2966,17 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H65" s="5" t="str">
         <f t="shared" ref="H65:H97" si="88">"sh ${check_script} ora2pg "&amp;UPPER(MID(E65,1,LEN(E65)-5))&amp;" ${dt}"</f>
@@ -2984,17 +2985,17 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H66" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3003,17 +3004,17 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H67" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3022,17 +3023,17 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H68" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3041,17 +3042,17 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H69" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3060,17 +3061,17 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H70" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3079,17 +3080,17 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H71" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3098,17 +3099,17 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H72" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3117,17 +3118,17 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H73" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3136,17 +3137,17 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H74" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3155,17 +3156,17 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H75" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3174,17 +3175,17 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H76" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3193,17 +3194,17 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H77" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3212,17 +3213,17 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H78" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3231,17 +3232,17 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H79" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3250,17 +3251,17 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H80" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3269,17 +3270,17 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H81" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3288,17 +3289,17 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H82" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3307,17 +3308,17 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H83" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3326,17 +3327,17 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H84" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3345,17 +3346,17 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H85" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3364,17 +3365,17 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H86" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3383,17 +3384,17 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H87" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3402,17 +3403,17 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H88" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3421,17 +3422,17 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H89" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3440,17 +3441,17 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H90" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3459,17 +3460,17 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H91" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3478,17 +3479,17 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H92" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3497,17 +3498,17 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H93" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3516,17 +3517,17 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H94" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3535,40 +3536,40 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I95" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H96" s="5" t="str">
         <f t="shared" si="88"/>
@@ -3577,45 +3578,45 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H97" s="5" t="str">
         <f t="shared" si="88"/>
         <v>sh ${check_script} ora2pg ORA2PG_DELETE_RE ${dt}</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>